<commit_message>
Formatting for input of JavaScript link
</commit_message>
<xml_diff>
--- a/CAR - Accessibility Review Template.xlsx
+++ b/CAR - Accessibility Review Template.xlsx
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="145">
   <si>
     <t>Complete?</t>
   </si>
@@ -550,6 +550,12 @@
   </si>
   <si>
     <t>Transcript Hours Needed</t>
+  </si>
+  <si>
+    <t>JavaScript Link</t>
+  </si>
+  <si>
+    <t>JavaScript links are frequently not accessible</t>
   </si>
 </sst>
 </file>
@@ -1476,6 +1482,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1550,15 +1565,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -1609,40 +1615,21 @@
     <cellStyle name="Total Hours" xfId="44"/>
     <cellStyle name="Total Hours 2" xfId="45"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="51">
     <dxf>
-      <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
+      <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1686,6 +1673,52 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF000000"/>
       </font>
@@ -1715,55 +1748,6 @@
           <bgColor theme="8"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -2082,22 +2066,22 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biweekly Time Sheet" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="52"/>
-      <tableStyleElement type="headerRow" dxfId="51"/>
-      <tableStyleElement type="lastColumn" dxfId="50"/>
+      <tableStyleElement type="wholeTable" dxfId="50"/>
+      <tableStyleElement type="headerRow" dxfId="49"/>
+      <tableStyleElement type="lastColumn" dxfId="48"/>
     </tableStyle>
     <tableStyle name="Table Style 1" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="49"/>
-      <tableStyleElement type="headerRow" dxfId="48"/>
+      <tableStyleElement type="wholeTable" dxfId="47"/>
+      <tableStyleElement type="headerRow" dxfId="46"/>
     </tableStyle>
     <tableStyle name="TableStyleMedium9 2" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="47"/>
-      <tableStyleElement type="headerRow" dxfId="46"/>
-      <tableStyleElement type="totalRow" dxfId="45"/>
-      <tableStyleElement type="firstColumn" dxfId="44"/>
-      <tableStyleElement type="lastColumn" dxfId="43"/>
-      <tableStyleElement type="firstRowStripe" dxfId="42"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="41"/>
+      <tableStyleElement type="wholeTable" dxfId="45"/>
+      <tableStyleElement type="headerRow" dxfId="44"/>
+      <tableStyleElement type="totalRow" dxfId="43"/>
+      <tableStyleElement type="firstColumn" dxfId="42"/>
+      <tableStyleElement type="lastColumn" dxfId="41"/>
+      <tableStyleElement type="firstRowStripe" dxfId="40"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="39"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -4269,21 +4253,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Issues" displayName="Issues" ref="B8:J142" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Issues" displayName="Issues" ref="B8:J142" dataDxfId="38">
   <autoFilter ref="B8:J142"/>
   <sortState ref="B9:K29">
     <sortCondition descending="1" ref="J8:J18"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="5" name="Completed?" totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="4" name="Location" dataDxfId="37" totalsRowDxfId="36" dataCellStyle="Heading 2"/>
-    <tableColumn id="2" name="Issue Type" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="11" name="Descriptive Errors " dataDxfId="33" totalsRowDxfId="32" dataCellStyle="Heading 2"/>
-    <tableColumn id="3" name="Notes" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="7" name="Severity *(1, 3, 5)" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="8" name="Occurrence *(1, 3, 5)" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="9" name="Detection *(1, 3, 5)" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="10" name="RPN*" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="5" name="Completed?" totalsRowLabel="Total" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="4" name="Location" dataDxfId="35" totalsRowDxfId="34" dataCellStyle="Heading 2"/>
+    <tableColumn id="2" name="Issue Type" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="11" name="Descriptive Errors " dataDxfId="31" totalsRowDxfId="30" dataCellStyle="Heading 2"/>
+    <tableColumn id="3" name="Notes" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="7" name="Severity *(1, 3, 5)" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="8" name="Occurrence *(1, 3, 5)" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="9" name="Detection *(1, 3, 5)" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="10" name="RPN*" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>Issues[[#This Row],[Severity *(1, 3, 5)]]*Issues[[#This Row],[Occurrence *(1, 3, 5)]]*Issues[[#This Row],[Detection *(1, 3, 5)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4292,15 +4276,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B3:I50" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B3:I50" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="B3:I50"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Element"/>
     <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="VideoID" dataDxfId="20"/>
+    <tableColumn id="3" name="VideoID" dataDxfId="15"/>
     <tableColumn id="4" name="Url"/>
-    <tableColumn id="5" name="VideoLength" dataDxfId="19"/>
-    <tableColumn id="6" name="Text" dataDxfId="18"/>
+    <tableColumn id="5" name="VideoLength" dataDxfId="14"/>
+    <tableColumn id="6" name="Text" dataDxfId="13"/>
     <tableColumn id="7" name="Transcript"/>
     <tableColumn id="8" name="MediaCount"/>
   </tableColumns>
@@ -4309,13 +4293,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="K3:L4" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="K3:L4" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="K3:L4"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Transcript Hours Needed" dataDxfId="3">
+    <tableColumn id="1" name="Transcript Hours Needed" dataDxfId="10">
       <calculatedColumnFormula>SUMIF(Table5[Transcript], "No", Table5[VideoLength])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Total Hours" dataDxfId="2">
+    <tableColumn id="2" name="Total Hours" dataDxfId="9">
       <calculatedColumnFormula>SUM(Table5[VideoLength])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4324,12 +4308,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57" displayName="Table57" ref="B3:D150" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57" displayName="Table57" ref="B3:D150" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B3:D150"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Location"/>
     <tableColumn id="2" name="URL"/>
-    <tableColumn id="3" name="Status" dataDxfId="16"/>
+    <tableColumn id="3" name="Status" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4343,7 +4327,7 @@
   </autoFilter>
   <tableColumns count="2">
     <tableColumn id="1" name="Issue Type" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Occurance" totalsRowFunction="sum" dataDxfId="15"/>
+    <tableColumn id="2" name="Occurance" totalsRowFunction="sum" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4353,8 +4337,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:C14" totalsRowShown="0">
   <autoFilter ref="B2:C14"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Complete?" dataDxfId="14"/>
-    <tableColumn id="2" name="Did you check?" dataDxfId="13"/>
+    <tableColumn id="1" name="Complete?" dataDxfId="1"/>
+    <tableColumn id="2" name="Did you check?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4654,7 +4638,7 @@
   <dimension ref="B1:L155"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4675,47 +4659,47 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
       <c r="E2" s="42"/>
-      <c r="F2" s="76" t="s">
+      <c r="F2" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="77"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="80"/>
     </row>
     <row r="3" spans="2:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21"/>
       <c r="C3" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
       <c r="G3" s="31"/>
       <c r="H3" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="82" t="s">
+      <c r="I3" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="83"/>
+      <c r="J3" s="86"/>
     </row>
     <row r="4" spans="2:12" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="57"/>
       <c r="C4" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="I4" s="25"/>
@@ -4726,11 +4710,11 @@
       <c r="C5" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
@@ -4752,17 +4736,17 @@
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="2:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="81" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="80"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="83"/>
     </row>
     <row r="8" spans="2:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
@@ -6947,28 +6931,28 @@
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" style="99" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="99" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="74" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="74" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" s="61" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="43"/>
       <c r="F1" s="73"/>
       <c r="G1" s="43"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="99"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
     </row>
     <row r="2" spans="2:12" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="89" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="88"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="91"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="69" t="s">
@@ -6995,74 +6979,74 @@
       <c r="I3" s="69" t="s">
         <v>136</v>
       </c>
-      <c r="K3" s="100" t="s">
+      <c r="K3" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="L3" s="101" t="s">
+      <c r="L3" s="76" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F4" s="99"/>
-      <c r="K4" s="99">
+      <c r="F4" s="74"/>
+      <c r="K4" s="74">
         <f>SUMIF(Table5[Transcript], "No", Table5[VideoLength])</f>
         <v>0</v>
       </c>
-      <c r="L4" s="99">
+      <c r="L4" s="74">
         <f>SUM(Table5[VideoLength])</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F5" s="99"/>
+      <c r="F5" s="74"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F6" s="99"/>
+      <c r="F6" s="74"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F7" s="99"/>
+      <c r="F7" s="74"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F8" s="99"/>
+      <c r="F8" s="74"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F9" s="99"/>
+      <c r="F9" s="74"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F10" s="99"/>
+      <c r="F10" s="74"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F11" s="99"/>
+      <c r="F11" s="74"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F12" s="99"/>
+      <c r="F12" s="74"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F13" s="99"/>
+      <c r="F13" s="74"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F14" s="99"/>
+      <c r="F14" s="74"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F15" s="99"/>
+      <c r="F15" s="74"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F16" s="99"/>
+      <c r="F16" s="74"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="99"/>
+      <c r="F17" s="74"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="99"/>
+      <c r="F18" s="74"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="99"/>
+      <c r="F19" s="74"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="99"/>
+      <c r="F20" s="74"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="99"/>
+      <c r="F21" s="74"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22" s="7"/>
@@ -7156,15 +7140,15 @@
     <mergeCell ref="B2:I2"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D50">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="Duplicate">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Duplicate">
       <formula>NOT(ISERROR(SEARCH("Duplicate",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G50">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Video not found">
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Video not found">
       <formula>NOT(ISERROR(SEARCH("Video not found",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Inline Media">
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="Inline Media">
       <formula>NOT(ISERROR(SEARCH("Inline Media",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7198,11 +7182,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="89" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="88"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="69" t="s">
@@ -7755,19 +7739,19 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:D3">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Duplicate Video">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Duplicate Video">
       <formula>NOT(ISERROR(SEARCH("Duplicate Video",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Video not found">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Video not found">
       <formula>NOT(ISERROR(SEARCH("Video not found",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Inline Media:&#10;Unable to find title or video length for this type of video">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Inline Media:&#10;Unable to find title or video length for this type of video">
       <formula>NOT(ISERROR(SEARCH("Inline Media:
 Unable to find title or video length for this type of video",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D150">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Duplicate">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Duplicate">
       <formula>NOT(ISERROR(SEARCH("Duplicate",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7796,10 +7780,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="90"/>
+      <c r="C2" s="93"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -7930,8 +7914,8 @@
   </sheetPr>
   <dimension ref="B2:S16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7957,119 +7941,119 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M2" s="91" t="s">
+      <c r="M2" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
-      <c r="S2" s="91"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
+      <c r="R2" s="94"/>
+      <c r="S2" s="94"/>
     </row>
     <row r="3" spans="2:19" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="94"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="94"/>
-      <c r="R3" s="94"/>
-      <c r="S3" s="94"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97"/>
+      <c r="O3" s="97"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
     </row>
     <row r="4" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="92"/>
-      <c r="Q4" s="92"/>
-      <c r="R4" s="92"/>
-      <c r="S4" s="92"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="95"/>
     </row>
     <row r="5" spans="2:19" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93" t="s">
+      <c r="C5" s="96"/>
+      <c r="D5" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93" t="s">
+      <c r="E5" s="96"/>
+      <c r="F5" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="93"/>
-      <c r="H5" s="93" t="s">
+      <c r="G5" s="96"/>
+      <c r="H5" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="93"/>
-      <c r="J5" s="93" t="s">
+      <c r="I5" s="96"/>
+      <c r="J5" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93" t="s">
+      <c r="K5" s="96"/>
+      <c r="L5" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="93"/>
-      <c r="N5" s="93" t="s">
+      <c r="M5" s="96"/>
+      <c r="N5" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="93"/>
-      <c r="P5" s="96" t="s">
+      <c r="O5" s="96"/>
+      <c r="P5" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" s="97"/>
-      <c r="R5" s="93" t="s">
+      <c r="Q5" s="100"/>
+      <c r="R5" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="S5" s="93"/>
+      <c r="S5" s="96"/>
     </row>
     <row r="6" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="92"/>
-      <c r="P6" s="92"/>
-      <c r="Q6" s="92"/>
-      <c r="R6" s="92"/>
-      <c r="S6" s="92"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="95"/>
+      <c r="S6" s="95"/>
     </row>
     <row r="7" spans="2:19" ht="298.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="64" t="s">
@@ -8204,8 +8188,12 @@
       <c r="M9" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="N9" s="64"/>
-      <c r="O9" s="68"/>
+      <c r="N9" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="O9" s="68" t="s">
+        <v>144</v>
+      </c>
       <c r="P9" s="65" t="s">
         <v>59</v>
       </c>
@@ -8506,11 +8494,11 @@
       <c r="C3" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="98" t="s">
+      <c r="E3" s="101" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
       <c r="I3" s="46" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Updated media total time formula
</commit_message>
<xml_diff>
--- a/CAR - Accessibility Review Template.xlsx
+++ b/CAR - Accessibility Review Template.xlsx
@@ -2159,7 +2159,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2547,9 +2546,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2650,7 +2647,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4310,7 +4306,7 @@
       <calculatedColumnFormula>SUMIF(Table5[Transcript], "No", Table5[VideoLength])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Total Hours" dataDxfId="9">
-      <calculatedColumnFormula>SUM(Table5[VideoLength])</calculatedColumnFormula>
+      <calculatedColumnFormula>SUMIF(Table5[VideoID],"&lt;&gt;*Duplicate Video*",Table5[VideoLength])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6926,7 +6922,7 @@
   <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7004,7 +7000,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="74">
-        <f>SUM(Table5[VideoLength])</f>
+        <f>SUMIF(Table5[VideoID],"&lt;&gt;*Duplicate Video*",Table5[VideoLength])</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>